<commit_message>
[feat] Inventory UI 추가
</commit_message>
<xml_diff>
--- a/SpartaFarming/Util/excel_files/Enum.xlsx
+++ b/SpartaFarming/Util/excel_files/Enum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sudo\Documents\GitHub\SpartaFarming\SpartaFarming\Util\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F5AFBD-B2B4-4CA3-8330-79A4BACCCFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA91A5B4-DA26-4A08-BE1C-CED684554E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9225" yWindow="4170" windowWidth="21720" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13770" yWindow="5160" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="시트1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>ItemType</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -38,15 +38,19 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Build</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Construction</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Food</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Weapon</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Seed</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -348,90 +352,99 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G1000"/>
+  <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="5" t="s">
+      <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>